<commit_message>
Latest data: Mon Aug 17 16:28:19 UTC 2020
</commit_message>
<xml_diff>
--- a/ON__ltc_dictionary__latest.xlsx
+++ b/ON__ltc_dictionary__latest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="6_{87EBC3B5-F512-4C0C-B881-F00D2CBACD90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{84DC9926-BC95-4D26-8946-DB91B0E345FA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93F082EE-1ADC-4ABF-AC67-F2F7B735D7CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,9 +15,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Variable Name</t>
   </si>
@@ -96,12 +94,6 @@
     <t>The values represent the total cumulative number of active cases among residents that resided in the home, regardless if they were transferred to a hospital.</t>
   </si>
   <si>
-    <t>Cumulative number of resident deaths in the Long-Term Care home as measured on "Report_Data_Extracted" date.</t>
-  </si>
-  <si>
-    <t>The values represent the total cumulative number of deaths among residents that resided in the home, regardless if they were transferred to a hospital.</t>
-  </si>
-  <si>
     <t>Total_LTC_HCW_Cases</t>
   </si>
   <si>
@@ -126,9 +118,6 @@
     <t>Nombre de foyers de soins de longue durée (SLD) déclarant une éclosion de COVID-19 en cours, établi à la date d'extraction des données des rapports.</t>
   </si>
   <si>
-    <t>Nombre actuel de cas actifs confirmés de COVID-19 parmi les résidents d’un foyer de soins de longue durée (SLD), établi à la date d'extraction des données des rapports.</t>
-  </si>
-  <si>
     <t>Nombre actuel de cas actifs confirmés de COVID-19 parmi le personnel d’un foyer de soins de longue durée (SLD), établi à la date d'extraction des données des rapports.</t>
   </si>
   <si>
@@ -147,9 +136,6 @@
     <t>Nombre cumulatif de cas positifs actifs de COVID-19 parmi les résidents du foyer de soins de longue durée, établi à la date d'extraction des données des rapports.</t>
   </si>
   <si>
-    <t>Nombre cumulatif de décès parmi les résidents du foyer de soins de longue durée, établi à la date d'extraction des données des rapports.</t>
-  </si>
-  <si>
     <t>Nombre de cas positifs actifs de COVID-19 parmi le personnel associé au foyer de soins de longue durée, établi à la date d'extraction des données des rapports.</t>
   </si>
   <si>
@@ -159,10 +145,26 @@
     <t>Les valeurs représentent le nombre cumulatif total de cas actifs parmi les résidents du foyer, peu importe leur hospitalisation le cas échéant.</t>
   </si>
   <si>
-    <t>Les valeurs représentent le nombre cumulatif total de décès parmi les résidents du foyer, peu importe leur hospitalisation le cas échéant.</t>
-  </si>
-  <si>
     <t>Les valeurs représentent le nombre cumulatif total de cas actifs parmi les employés qui ont travaillé au foyer, peu importe leur hospitalisation le cas échéant.</t>
+  </si>
+  <si>
+    <t>LTC_City</t>
+  </si>
+  <si>
+    <t>Official city of the Long-Term Care (LTC) home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Ville officielle du foyer de soins de longue durée (SLD).</t>
+  </si>
+  <si>
+    <t>LTC_Homes_With_Resolved_Outbrea</t>
+  </si>
+  <si>
+    <t>Number of Long-Term Care (LTC) homes reporting a resolved COVID-19 outbreak as measured on the "Report_Data_Extracted" date.</t>
+  </si>
+  <si>
+    <t>Nombre de foyers de soins de longue durée (SLD) déclarant une éclosion de COVID-19 résolue, établi à la date d'extraction des données des rapports.</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1040,19 +1042,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1066,13 +1068,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1086,189 +1088,481 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>45</v>
+      <c r="F13" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010066B7C8A6783BDE48A0D096D986242705" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4dff437761093b902986445f837b2de4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8022163d-7682-4450-abe1-587ac0f6376b" xmlns:ns4="ef354a9c-7d37-4f03-a7ba-bf428376f60d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5750bee1cb0039862374ebed3f7b4465" ns3:_="" ns4:_="">
+    <xsd:import namespace="8022163d-7682-4450-abe1-587ac0f6376b"/>
+    <xsd:import namespace="ef354a9c-7d37-4f03-a7ba-bf428376f60d"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8022163d-7682-4450-abe1-587ac0f6376b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ef354a9c-7d37-4f03-a7ba-bf428376f60d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905AAD1C-7A2D-4E2E-A986-D1468E461ABF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8022163d-7682-4450-abe1-587ac0f6376b"/>
+    <ds:schemaRef ds:uri="ef354a9c-7d37-4f03-a7ba-bf428376f60d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BB26B03-6CD8-4D9D-8307-2CBE12BEDF55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ACADE45-6CD9-4449-86A2-B43AC7FA4C46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8022163d-7682-4450-abe1-587ac0f6376b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef354a9c-7d37-4f03-a7ba-bf428376f60d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Latest data: Tue Nov 10 19:28:15 UTC 2020
</commit_message>
<xml_diff>
--- a/ON__ltc_dictionary__latest.xlsx
+++ b/ON__ltc_dictionary__latest.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93F082EE-1ADC-4ABF-AC67-F2F7B735D7CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="6_{E0E79AC6-42BA-4E35-B71B-B1E10D3B6004}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B1213589-3AE3-4A12-9CE6-7F2F7EA0117D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4935" yWindow="9570" windowWidth="28065" windowHeight="9495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTC_Dictionary" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Variable Name</t>
   </si>
@@ -31,18 +31,12 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>Additional Notes</t>
-  </si>
-  <si>
     <t>Report_Data_Extracted</t>
   </si>
   <si>
     <t>The data is extracted from the Ministry of Long-Term Care (MLTC) system each day in the afternoon.</t>
   </si>
   <si>
-    <t>Data is self-reported by the long-term care homes (the homes) to the Ministry of Long-Term Care (MLTC). Daily case and death figures may not immediately match the numbers posted by the local public health units (i.e. iPHIS database) due to lags in reporting time.</t>
-  </si>
-  <si>
     <t xml:space="preserve">LTC_Homes_With_Active_Outbreak </t>
   </si>
   <si>
@@ -91,27 +85,18 @@
     <t>Number of active Cumulative COVID-19 positive cases among residents of the Long-Term Care home as measured on "Report_Data_Extracted" date.</t>
   </si>
   <si>
-    <t>The values represent the total cumulative number of active cases among residents that resided in the home, regardless if they were transferred to a hospital.</t>
-  </si>
-  <si>
     <t>Total_LTC_HCW_Cases</t>
   </si>
   <si>
     <t>Number of active COVID-19 positive cases among staff associated with the Long-Term Care home as measured on "Report_Data_Extracted" date.</t>
   </si>
   <si>
-    <t>The values represent the total cumulative number of active cases among staff that worked in the home, regardless if they were transferred to a hospital.</t>
-  </si>
-  <si>
     <t>Nom de la variable</t>
   </si>
   <si>
     <t>Définition</t>
   </si>
   <si>
-    <t>Notes additionnelles</t>
-  </si>
-  <si>
     <t>Les données sont extraites du système du ministère des Soins de longue durée (MSLD) chaque jour en après-midi.</t>
   </si>
   <si>
@@ -137,15 +122,6 @@
   </si>
   <si>
     <t>Nombre de cas positifs actifs de COVID-19 parmi le personnel associé au foyer de soins de longue durée, établi à la date d'extraction des données des rapports.</t>
-  </si>
-  <si>
-    <t>Les foyers de soins de longue durée communiquent eux-mêmes les données au ministère des Soins de longue durée (MSLD). Les chiffres quotidiens des cas et des décès peuvent ne pas correspondre immédiatement aux chiffres publiés par les bureaux locaux de santé publique (c.-à-d. la base de données du SIISP) en raison d’un décalage dans les heures de déclaration.</t>
-  </si>
-  <si>
-    <t>Les valeurs représentent le nombre cumulatif total de cas actifs parmi les résidents du foyer, peu importe leur hospitalisation le cas échéant.</t>
-  </si>
-  <si>
-    <t>Les valeurs représentent le nombre cumulatif total de cas actifs parmi les employés qui ont travaillé au foyer, peu importe leur hospitalisation le cas échéant.</t>
   </si>
   <si>
     <t>LTC_City</t>
@@ -655,15 +631,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1022,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,535 +1007,192 @@
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" customWidth="1"/>
     <col min="4" max="4" width="55.42578125" customWidth="1"/>
-    <col min="5" max="6" width="63.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010066B7C8A6783BDE48A0D096D986242705" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4dff437761093b902986445f837b2de4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8022163d-7682-4450-abe1-587ac0f6376b" xmlns:ns4="ef354a9c-7d37-4f03-a7ba-bf428376f60d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5750bee1cb0039862374ebed3f7b4465" ns3:_="" ns4:_="">
-    <xsd:import namespace="8022163d-7682-4450-abe1-587ac0f6376b"/>
-    <xsd:import namespace="ef354a9c-7d37-4f03-a7ba-bf428376f60d"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8022163d-7682-4450-abe1-587ac0f6376b" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ef354a9c-7d37-4f03-a7ba-bf428376f60d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905AAD1C-7A2D-4E2E-A986-D1468E461ABF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8022163d-7682-4450-abe1-587ac0f6376b"/>
-    <ds:schemaRef ds:uri="ef354a9c-7d37-4f03-a7ba-bf428376f60d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BB26B03-6CD8-4D9D-8307-2CBE12BEDF55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ACADE45-6CD9-4449-86A2-B43AC7FA4C46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="8022163d-7682-4450-abe1-587ac0f6376b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ef354a9c-7d37-4f03-a7ba-bf428376f60d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Latest data: Wed Nov 25 16:51:48 UTC 2020
</commit_message>
<xml_diff>
--- a/ON__ltc_dictionary__latest.xlsx
+++ b/ON__ltc_dictionary__latest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="6_{E0E79AC6-42BA-4E35-B71B-B1E10D3B6004}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B1213589-3AE3-4A12-9CE6-7F2F7EA0117D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD5894-5992-463B-9B0E-CA4D43458962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="9570" windowWidth="28065" windowHeight="9495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTC_Dictionary" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Variable Name</t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t>Nombre de foyers de soins de longue durée (SLD) déclarant une éclosion de COVID-19 résolue, établi à la date d'extraction des données des rapports.</t>
+  </si>
+  <si>
+    <t>PHU_Num</t>
+  </si>
+  <si>
+    <t>PHU</t>
+  </si>
+  <si>
+    <t>ID of the Public Health Unit (PHU) region in which the long term care home is located.</t>
+  </si>
+  <si>
+    <t>Name of the Public Health Unit (PHU) region in which the long term care home is located.</t>
+  </si>
+  <si>
+    <t>ID de la région du bureau de santé publique dans laquelle se trouve le foyer de soins de longue durée.</t>
+  </si>
+  <si>
+    <t>Nom de la région du bureau de santé publique dans laquelle se trouve le foyer de soins de longue durée.</t>
   </si>
 </sst>
 </file>
@@ -631,7 +649,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -640,6 +658,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -995,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,73 +1145,101 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>